<commit_message>
Update Leave Card 1/19/2024 4:44 pm
</commit_message>
<xml_diff>
--- a/CASUAL/LA CITY MARKET/BRON, FLORENCIO.xlsx
+++ b/CASUAL/LA CITY MARKET/BRON, FLORENCIO.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="2"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTION" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="95">
   <si>
     <t>PERIOD</t>
   </si>
@@ -319,6 +319,9 @@
   </si>
   <si>
     <t>12/03,08,12/2023</t>
+  </si>
+  <si>
+    <t>2024</t>
   </si>
 </sst>
 </file>
@@ -1253,7 +1256,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1296,7 +1299,7 @@
         <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1360,7 +1363,7 @@
         <xdr:cNvPr id="4" name="Arrow: Left 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1420,7 +1423,7 @@
         <xdr:cNvPr id="8" name="Oval 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1486,7 +1489,7 @@
         <xdr:cNvPr id="9" name="Arrow: Left-Right 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1549,7 +1552,7 @@
         <xdr:cNvPr id="10" name="TextBox 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1647,7 +1650,7 @@
         <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1706,7 +1709,7 @@
         <xdr:cNvPr id="19" name="TextBox 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1771,7 +1774,7 @@
         <xdr:cNvPr id="20" name="Picture 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1814,7 +1817,7 @@
         <xdr:cNvPr id="21" name="TextBox 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1889,7 +1892,7 @@
         <xdr:cNvPr id="22" name="TextBox 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2075,7 +2078,7 @@
         <xdr:cNvPr id="23" name="Oval 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2141,7 +2144,7 @@
         <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2199,7 +2202,7 @@
         <xdr:cNvPr id="26" name="Oval 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2265,7 +2268,7 @@
         <xdr:cNvPr id="27" name="Straight Arrow Connector 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2321,7 +2324,7 @@
         <xdr:cNvPr id="30" name="TextBox 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2396,7 +2399,7 @@
         <xdr:cNvPr id="31" name="Picture 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2439,7 +2442,7 @@
         <xdr:cNvPr id="32" name="Oval 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2505,7 +2508,7 @@
         <xdr:cNvPr id="33" name="Straight Arrow Connector 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2561,7 +2564,7 @@
         <xdr:cNvPr id="34" name="TextBox 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2657,7 +2660,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A8:K137" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A8:K138" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <tableColumns count="11">
     <tableColumn id="1" name="PERIOD" dataDxfId="25"/>
     <tableColumn id="2" name="PARTICULARS" dataDxfId="24"/>
@@ -3034,12 +3037,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:K137"/>
+  <dimension ref="A2:K138"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3690" topLeftCell="A82" activePane="bottomLeft"/>
       <selection activeCell="I10" sqref="I10"/>
-      <selection pane="bottomLeft" activeCell="C93" sqref="C93"/>
+      <selection pane="bottomLeft" activeCell="J97" sqref="J97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3200,7 +3203,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="13">
         <f>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])</f>
-        <v>51.942999999999998</v>
+        <v>54.442999999999998</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="13" t="str">
@@ -3210,7 +3213,7 @@
       <c r="H9" s="11"/>
       <c r="I9" s="13">
         <f>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])</f>
-        <v>87.5</v>
+        <v>89</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
@@ -4966,13 +4969,15 @@
         <v>45231</v>
       </c>
       <c r="B94" s="20"/>
-      <c r="C94" s="13"/>
+      <c r="C94" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D94" s="39"/>
       <c r="E94" s="9"/>
       <c r="F94" s="20"/>
-      <c r="G94" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G94" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H94" s="39"/>
       <c r="I94" s="9"/>
@@ -4984,13 +4989,15 @@
         <v>45261</v>
       </c>
       <c r="B95" s="20"/>
-      <c r="C95" s="13"/>
+      <c r="C95" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D95" s="39"/>
       <c r="E95" s="9"/>
       <c r="F95" s="20"/>
-      <c r="G95" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G95" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H95" s="39"/>
       <c r="I95" s="9"/>
@@ -4998,7 +5005,9 @@
       <c r="K95" s="20"/>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A96" s="40"/>
+      <c r="A96" s="48" t="s">
+        <v>94</v>
+      </c>
       <c r="B96" s="20"/>
       <c r="C96" s="13"/>
       <c r="D96" s="39"/>
@@ -5014,23 +5023,30 @@
       <c r="K96" s="20"/>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A97" s="40"/>
-      <c r="B97" s="20"/>
+      <c r="A97" s="40">
+        <v>45292</v>
+      </c>
+      <c r="B97" s="20" t="s">
+        <v>56</v>
+      </c>
       <c r="C97" s="13"/>
       <c r="D97" s="39"/>
       <c r="E97" s="9"/>
       <c r="F97" s="20"/>
-      <c r="G97" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H97" s="39"/>
+      <c r="G97" s="13"/>
+      <c r="H97" s="39">
+        <v>1</v>
+      </c>
       <c r="I97" s="9"/>
       <c r="J97" s="11"/>
-      <c r="K97" s="20"/>
+      <c r="K97" s="49">
+        <v>45300</v>
+      </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A98" s="40"/>
+      <c r="A98" s="40">
+        <v>45323</v>
+      </c>
       <c r="B98" s="20"/>
       <c r="C98" s="13"/>
       <c r="D98" s="39"/>
@@ -5046,7 +5062,9 @@
       <c r="K98" s="20"/>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A99" s="40"/>
+      <c r="A99" s="40">
+        <v>45352</v>
+      </c>
       <c r="B99" s="20"/>
       <c r="C99" s="13"/>
       <c r="D99" s="39"/>
@@ -5062,7 +5080,9 @@
       <c r="K99" s="20"/>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A100" s="40"/>
+      <c r="A100" s="40">
+        <v>45383</v>
+      </c>
       <c r="B100" s="20"/>
       <c r="C100" s="13"/>
       <c r="D100" s="39"/>
@@ -5078,7 +5098,9 @@
       <c r="K100" s="20"/>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A101" s="40"/>
+      <c r="A101" s="40">
+        <v>45413</v>
+      </c>
       <c r="B101" s="20"/>
       <c r="C101" s="13"/>
       <c r="D101" s="39"/>
@@ -5094,7 +5116,9 @@
       <c r="K101" s="20"/>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A102" s="40"/>
+      <c r="A102" s="40">
+        <v>45444</v>
+      </c>
       <c r="B102" s="20"/>
       <c r="C102" s="13"/>
       <c r="D102" s="39"/>
@@ -5110,7 +5134,9 @@
       <c r="K102" s="20"/>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A103" s="40"/>
+      <c r="A103" s="40">
+        <v>45474</v>
+      </c>
       <c r="B103" s="20"/>
       <c r="C103" s="13"/>
       <c r="D103" s="39"/>
@@ -5126,7 +5152,9 @@
       <c r="K103" s="20"/>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A104" s="40"/>
+      <c r="A104" s="40">
+        <v>45505</v>
+      </c>
       <c r="B104" s="20"/>
       <c r="C104" s="13"/>
       <c r="D104" s="39"/>
@@ -5142,7 +5170,9 @@
       <c r="K104" s="20"/>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A105" s="40"/>
+      <c r="A105" s="40">
+        <v>45536</v>
+      </c>
       <c r="B105" s="20"/>
       <c r="C105" s="13"/>
       <c r="D105" s="39"/>
@@ -5158,7 +5188,9 @@
       <c r="K105" s="20"/>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A106" s="40"/>
+      <c r="A106" s="40">
+        <v>45566</v>
+      </c>
       <c r="B106" s="20"/>
       <c r="C106" s="13"/>
       <c r="D106" s="39"/>
@@ -5174,7 +5206,9 @@
       <c r="K106" s="20"/>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A107" s="40"/>
+      <c r="A107" s="40">
+        <v>45597</v>
+      </c>
       <c r="B107" s="20"/>
       <c r="C107" s="13"/>
       <c r="D107" s="39"/>
@@ -5654,20 +5688,36 @@
       <c r="K136" s="20"/>
     </row>
     <row r="137" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A137" s="41"/>
-      <c r="B137" s="15"/>
-      <c r="C137" s="42"/>
-      <c r="D137" s="43"/>
+      <c r="A137" s="40"/>
+      <c r="B137" s="20"/>
+      <c r="C137" s="13"/>
+      <c r="D137" s="39"/>
       <c r="E137" s="9"/>
-      <c r="F137" s="15"/>
-      <c r="G137" s="42" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H137" s="43"/>
+      <c r="F137" s="20"/>
+      <c r="G137" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H137" s="39"/>
       <c r="I137" s="9"/>
-      <c r="J137" s="12"/>
-      <c r="K137" s="15"/>
+      <c r="J137" s="11"/>
+      <c r="K137" s="20"/>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A138" s="41"/>
+      <c r="B138" s="15"/>
+      <c r="C138" s="42"/>
+      <c r="D138" s="43"/>
+      <c r="E138" s="9"/>
+      <c r="F138" s="15"/>
+      <c r="G138" s="42" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H138" s="43"/>
+      <c r="I138" s="9"/>
+      <c r="J138" s="12"/>
+      <c r="K138" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -5716,7 +5766,7 @@
   </sheetPr>
   <dimension ref="A2:K101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3690" topLeftCell="A40" activePane="bottomLeft"/>
       <selection activeCell="I9" sqref="I9"/>
       <selection pane="bottomLeft" activeCell="F59" sqref="F59"/>
@@ -7699,17 +7749,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:J7"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="J3:K3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:J7"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">

</xml_diff>